<commit_message>
update table selection, date format
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="45">
   <si>
     <t>Id</t>
   </si>
@@ -42,7 +42,31 @@
     <t>Warehouse id</t>
   </si>
   <si>
-    <t>gergertg</t>
+    <t>Bia heniken</t>
+  </si>
+  <si>
+    <t>BIA</t>
+  </si>
+  <si>
+    <t>Heniken</t>
+  </si>
+  <si>
+    <t>KHO HO CHI MINH</t>
+  </si>
+  <si>
+    <t>Bia Saigon</t>
+  </si>
+  <si>
+    <t>KHO DA NANG</t>
+  </si>
+  <si>
+    <t>Bia Ha Noi</t>
+  </si>
+  <si>
+    <t>KhO HAI PHONG</t>
+  </si>
+  <si>
+    <t>Cigar box 10</t>
   </si>
   <si>
     <t>THUOC LA</t>
@@ -51,37 +75,79 @@
     <t>Cohiba</t>
   </si>
   <si>
+    <t>KhO HAI DUONG</t>
+  </si>
+  <si>
+    <t>Cigar box 21</t>
+  </si>
+  <si>
+    <t>0025-10-11T00:00:00</t>
+  </si>
+  <si>
+    <t>KhO CAM RANH</t>
+  </si>
+  <si>
+    <t>Cutter Cigar</t>
+  </si>
+  <si>
     <t>KHO HA NOI</t>
   </si>
   <si>
-    <t>Bia heniken</t>
+    <t>BMW 320i</t>
+  </si>
+  <si>
+    <t>OTO</t>
+  </si>
+  <si>
+    <t>BMW</t>
+  </si>
+  <si>
+    <t>BMW s1000rr</t>
+  </si>
+  <si>
+    <t>BMW 520i</t>
+  </si>
+  <si>
+    <t>Chat no ran</t>
+  </si>
+  <si>
+    <t>TNT</t>
+  </si>
+  <si>
+    <t>Chat no deo</t>
+  </si>
+  <si>
+    <t>Kip no TNT</t>
+  </si>
+  <si>
+    <t>Cohiba Special</t>
+  </si>
+  <si>
+    <t>0025-10-12T00:00:00</t>
   </si>
   <si>
     <t>RUOU</t>
   </si>
   <si>
-    <t>TNT</t>
-  </si>
-  <si>
-    <t>Cigar Cohiba</t>
-  </si>
-  <si>
-    <t>BIA</t>
-  </si>
-  <si>
-    <t>Heniken</t>
-  </si>
-  <si>
-    <t>KHO HO CHI MINH</t>
-  </si>
-  <si>
-    <t>VAT LIEU NO CONG NGHIEP</t>
-  </si>
-  <si>
-    <t>KHO DA NANG</t>
-  </si>
-  <si>
-    <t>Airbus A320</t>
+    <t>moto BMW 1200cc</t>
+  </si>
+  <si>
+    <t>Strongbow</t>
+  </si>
+  <si>
+    <t>Corona</t>
+  </si>
+  <si>
+    <t>Malboro</t>
+  </si>
+  <si>
+    <t>Thang long</t>
+  </si>
+  <si>
+    <t>thuoc la 555</t>
+  </si>
+  <si>
+    <t>0025-10-14T00:00:00</t>
   </si>
   <si>
     <t>Evaluation Only. Created with Aspose.Cells for Java.Copyright 2003 - 2016 Aspose Pty Ltd.</t>
@@ -555,18 +621,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="2.7142857142857144" customWidth="1"/>
-    <col min="2" max="2" width="11.857142857142858" customWidth="1"/>
-    <col min="3" max="3" width="7.285714285714286" customWidth="1"/>
-    <col min="4" max="4" width="10.714285714285714" customWidth="1"/>
+    <col min="1" max="1" width="3.2857142857142856" customWidth="1"/>
+    <col min="2" max="2" width="17.285714285714285" customWidth="1"/>
+    <col min="3" max="3" width="11.285714285714286" customWidth="1"/>
+    <col min="4" max="4" width="18.571428571428573" customWidth="1"/>
     <col min="5" max="5" width="7.714285714285714" customWidth="1"/>
-    <col min="6" max="6" width="26.285714285714285" customWidth="1"/>
+    <col min="6" max="6" width="10.714285714285714" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
     <col min="8" max="8" width="17.285714285714285" customWidth="1"/>
   </cols>
@@ -599,19 +665,19 @@
     </row>
     <row r="2" spans="1:8" ht="12.75">
       <c r="A2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
       <c r="C2">
-        <v>676447</v>
+        <v>20000</v>
       </c>
       <c r="D2">
-        <v>154353</v>
+        <v>43532</v>
       </c>
       <c r="E2">
-        <v>78</v>
+        <v>800</v>
       </c>
       <c r="F2" t="s">
         <v>9</v>
@@ -625,65 +691,65 @@
     </row>
     <row r="3" spans="1:8" ht="12.75">
       <c r="A3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
       </c>
       <c r="C3">
-        <v>10000</v>
+        <v>16000</v>
       </c>
       <c r="D3">
-        <v>43532</v>
+        <v>43941</v>
       </c>
       <c r="E3">
-        <v>500</v>
+        <v>900</v>
       </c>
       <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" t="s">
         <v>13</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="12.75">
       <c r="A4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4">
-        <v>800000</v>
+        <v>10000</v>
       </c>
       <c r="D4">
         <v>43941</v>
       </c>
       <c r="E4">
-        <v>300</v>
+        <v>1000</v>
       </c>
       <c r="F4" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="G4" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="H4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="12.75">
       <c r="A5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C5">
-        <v>800000</v>
+        <v>600000</v>
       </c>
       <c r="D5">
         <v>43941</v>
@@ -692,65 +758,403 @@
         <v>300</v>
       </c>
       <c r="F5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" t="s">
         <v>19</v>
-      </c>
-      <c r="G5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="12.75">
       <c r="A6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C6">
-        <v>800000</v>
-      </c>
-      <c r="D6">
-        <v>43941</v>
+        <v>2000000</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
       </c>
       <c r="E6">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="F6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H6" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="12.75">
       <c r="A7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C7">
-        <v>800000</v>
+        <v>300000</v>
       </c>
       <c r="D7">
         <v>43941</v>
       </c>
       <c r="E7">
+        <v>500</v>
+      </c>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="12.75">
+      <c r="A8">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8">
+        <v>1000000000</v>
+      </c>
+      <c r="D8">
+        <v>43941</v>
+      </c>
+      <c r="E8">
+        <v>16</v>
+      </c>
+      <c r="F8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="12.75">
+      <c r="A9">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9">
+        <v>600000000</v>
+      </c>
+      <c r="D9">
+        <v>43941</v>
+      </c>
+      <c r="E9">
+        <v>20</v>
+      </c>
+      <c r="F9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="12.75">
+      <c r="A10">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10">
+        <v>2000000000</v>
+      </c>
+      <c r="D10">
+        <v>43941</v>
+      </c>
+      <c r="E10">
+        <v>11</v>
+      </c>
+      <c r="F10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="12.75">
+      <c r="A11">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11">
+        <v>9000000</v>
+      </c>
+      <c r="D11">
+        <v>43941</v>
+      </c>
+      <c r="E11">
+        <v>610</v>
+      </c>
+      <c r="F11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" t="s">
+        <v>31</v>
+      </c>
+      <c r="H11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="12.75">
+      <c r="A12">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12">
+        <v>200000000</v>
+      </c>
+      <c r="D12">
+        <v>43941</v>
+      </c>
+      <c r="E12">
+        <v>390</v>
+      </c>
+      <c r="F12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" t="s">
+        <v>31</v>
+      </c>
+      <c r="H12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="12.75">
+      <c r="A13">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13">
+        <v>2000000</v>
+      </c>
+      <c r="D13">
+        <v>43941</v>
+      </c>
+      <c r="E13">
         <v>300</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" t="s">
+        <v>31</v>
+      </c>
+      <c r="H13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="12.75">
+      <c r="A14">
+        <v>21</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14">
+        <v>300000</v>
+      </c>
+      <c r="D14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14">
+        <v>30</v>
+      </c>
+      <c r="F14" t="s">
+        <v>36</v>
+      </c>
+      <c r="G14" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="12.75">
+      <c r="A15">
+        <v>22</v>
+      </c>
+      <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15">
+        <v>1000000000</v>
+      </c>
+      <c r="D15">
+        <v>43210</v>
+      </c>
+      <c r="E15">
+        <v>6</v>
+      </c>
+      <c r="F15" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" t="s">
+        <v>27</v>
+      </c>
+      <c r="H15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="12.75">
+      <c r="A16">
+        <v>23</v>
+      </c>
+      <c r="B16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16">
+        <v>20000</v>
+      </c>
+      <c r="D16">
+        <v>43924</v>
+      </c>
+      <c r="E16">
+        <v>200</v>
+      </c>
+      <c r="F16" t="s">
+        <v>36</v>
+      </c>
+      <c r="G16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="12.75">
+      <c r="A17">
+        <v>24</v>
+      </c>
+      <c r="B17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17">
+        <v>50000</v>
+      </c>
+      <c r="D17">
+        <v>44820</v>
+      </c>
+      <c r="E17">
+        <v>500</v>
+      </c>
+      <c r="F17" t="s">
         <v>9</v>
       </c>
-      <c r="G7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H7" t="s">
-        <v>20</v>
+      <c r="G17" t="s">
+        <v>10</v>
+      </c>
+      <c r="H17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="12.75">
+      <c r="A18">
+        <v>25</v>
+      </c>
+      <c r="B18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18">
+        <v>30000</v>
+      </c>
+      <c r="D18">
+        <v>44672</v>
+      </c>
+      <c r="E18">
+        <v>200</v>
+      </c>
+      <c r="F18" t="s">
+        <v>17</v>
+      </c>
+      <c r="G18" t="s">
+        <v>18</v>
+      </c>
+      <c r="H18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="12.75">
+      <c r="A19">
+        <v>26</v>
+      </c>
+      <c r="B19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19">
+        <v>10000</v>
+      </c>
+      <c r="D19">
+        <v>44915</v>
+      </c>
+      <c r="E19">
+        <v>1000</v>
+      </c>
+      <c r="F19" t="s">
+        <v>17</v>
+      </c>
+      <c r="G19" t="s">
+        <v>18</v>
+      </c>
+      <c r="H19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="12.75">
+      <c r="A20">
+        <v>27</v>
+      </c>
+      <c r="B20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20">
+        <v>50000</v>
+      </c>
+      <c r="D20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20">
+        <v>400</v>
+      </c>
+      <c r="F20" t="s">
+        <v>17</v>
+      </c>
+      <c r="G20" t="s">
+        <v>18</v>
+      </c>
+      <c r="H20" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -769,7 +1173,7 @@
   <sheetData>
     <row r="5" ht="23.25" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>